<commit_message>
this is newly modified code
</commit_message>
<xml_diff>
--- a/src/test/java/com/OrangeHrm/testData/LoginData.xlsx
+++ b/src/test/java/com/OrangeHrm/testData/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\OrangeHrmProject\src\test\java\com\OrangeHrm\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB46F0A2-6A1F-4835-BB89-8335428B0BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB73AD42-834E-4580-9D55-AC2A9222309D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6884A388-922B-4CB1-A670-10D41100E8B7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Username</t>
   </si>
@@ -45,25 +45,19 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>admin</t>
-  </si>
-  <si>
     <t>minadq</t>
   </si>
   <si>
-    <t>gashghj</t>
-  </si>
-  <si>
     <t>admin123</t>
   </si>
   <si>
-    <t>jshsbgsg</t>
-  </si>
-  <si>
     <t>radmun</t>
   </si>
   <si>
-    <t>bhhbagg</t>
+    <t>skijwjh</t>
+  </si>
+  <si>
+    <t>abbmin</t>
   </si>
 </sst>
 </file>
@@ -440,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D6A350-57BE-489A-939F-14DC687C1BB1}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="A1:XFD1048576"/>
+      <selection activeCell="B1" sqref="A1:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -464,28 +458,28 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -493,10 +487,13 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
+      </c>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -504,8 +501,6 @@
     <hyperlink ref="B2" r:id="rId1" display="admin123@" xr:uid="{39F534CC-05A1-487E-A42C-9446A44BF1CF}"/>
     <hyperlink ref="B3" r:id="rId2" display="radmun@" xr:uid="{3D7FCA4E-3346-4E1F-87B5-790DFF8EC6CD}"/>
     <hyperlink ref="B4" r:id="rId3" display="jshsbgsg@" xr:uid="{906AAB21-73B6-401E-9EFC-72EC47576EEA}"/>
-    <hyperlink ref="B5" r:id="rId4" display="admin123@" xr:uid="{8EB1C6CF-C7D6-4A8D-B048-513CF77F2985}"/>
-    <hyperlink ref="B6" r:id="rId5" display="bhhbagg@" xr:uid="{FBE41DB2-1288-4119-B3AC-EE3ABFDC0377}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>